<commit_message>
Added in a random examples of statistical neighbours, have made LA 2 stat neighbour reactive to LA 1, added LAIT info
</commit_message>
<xml_diff>
--- a/data/10_Demographics.xlsx
+++ b/data/10_Demographics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/muireann_settle_education_gov_uk/Documents/Documents/Projects (R)/childrens_social_services_offenders_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B7A830354C60D8073ABC5D7D78F9843DC9D0B195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23B8C29-0D47-4E5A-AF71-7226220457E3}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_B7A830354C60D8073ABC5D7D78F9843DC9D0B195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675047C3-FD5A-44DC-9E1B-EE14F9C1C39A}"/>
   <bookViews>
-    <workbookView xWindow="-27810" yWindow="1185" windowWidth="15330" windowHeight="12315" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info_table" sheetId="1" r:id="rId1"/>
@@ -1531,9 +1531,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -10477,9 +10482,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -11777,7 +11788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -12223,6 +12234,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="22.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Error with package 'checkmate', ran renv::hydrate()
</commit_message>
<xml_diff>
--- a/data/10_Demographics.xlsx
+++ b/data/10_Demographics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/muireann_settle_education_gov_uk/Documents/Documents/Projects (R)/childrens_social_services_offenders_dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_B7A830354C60D8073ABC5D7D78F9843DC9D0B195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675047C3-FD5A-44DC-9E1B-EE14F9C1C39A}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_B7A830354C60D8073ABC5D7D78F9843DC9D0B195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33129F9-B084-4FC3-94A6-3C6243E71874}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info_table" sheetId="1" r:id="rId1"/>
@@ -909,9 +909,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -1531,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed tibble() function in stat neighbour data
</commit_message>
<xml_diff>
--- a/data/10_Demographics.xlsx
+++ b/data/10_Demographics.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="7" documentId="11_B7A830354C60D8073ABC5D7D78F9843DC9D0B195" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33129F9-B084-4FC3-94A6-3C6243E71874}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info_table" sheetId="1" r:id="rId1"/>
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3619,7 +3619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E421"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -12244,7 +12246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>